<commit_message>
Changes made during episode 12
</commit_message>
<xml_diff>
--- a/doc/ItemPlanning.xlsx
+++ b/doc/ItemPlanning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\_BC\streamRepos\Biggening\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BA01B15-53FE-47C7-A620-DF5BD52CA9DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA009F16-7249-4C79-950A-70507FD7F1BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2100" yWindow="3585" windowWidth="20475" windowHeight="10395" xr2:uid="{8D42B13D-5ABD-42CE-A22D-5C49C32B1F1D}"/>
+    <workbookView xWindow="2025" yWindow="3555" windowWidth="24945" windowHeight="11385" xr2:uid="{8D42B13D-5ABD-42CE-A22D-5C49C32B1F1D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -92,9 +92,6 @@
     <t>CLASS3</t>
   </si>
   <si>
-    <t>2001;1</t>
-  </si>
-  <si>
     <t>BOM</t>
   </si>
   <si>
@@ -102,6 +99,9 @@
   </si>
   <si>
     <t>10;20;30</t>
+  </si>
+  <si>
+    <t>2001,1;2002,1</t>
   </si>
 </sst>
 </file>
@@ -456,7 +456,7 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,10 +499,10 @@
         <v>8</v>
       </c>
       <c r="K1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" t="s">
         <v>20</v>
-      </c>
-      <c r="L1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -561,6 +561,9 @@
       <c r="D4" t="s">
         <v>16</v>
       </c>
+      <c r="E4">
+        <v>20</v>
+      </c>
       <c r="G4">
         <v>3</v>
       </c>
@@ -591,10 +594,10 @@
         <v>1</v>
       </c>
       <c r="K5" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes during Episode 14
</commit_message>
<xml_diff>
--- a/doc/ItemPlanning.xlsx
+++ b/doc/ItemPlanning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\_BC\streamRepos\Biggening\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA009F16-7249-4C79-950A-70507FD7F1BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9412F9A-B695-4CBC-BE8B-2328A9D56770}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2025" yWindow="3555" windowWidth="24945" windowHeight="11385" xr2:uid="{8D42B13D-5ABD-42CE-A22D-5C49C32B1F1D}"/>
   </bookViews>
@@ -101,7 +101,7 @@
     <t>10;20;30</t>
   </si>
   <si>
-    <t>2001,1;2002,1</t>
+    <t>2001,55;2002,77</t>
   </si>
 </sst>
 </file>
@@ -456,7 +456,7 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>